<commit_message>
uploaded the rest of the visualizations
</commit_message>
<xml_diff>
--- a/3.14.Confidence-intervals.Two-means.Independent-samples-Part-1-exercise.xlsx
+++ b/3.14.Confidence-intervals.Two-means.Independent-samples-Part-1-exercise.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9739E972-2381-0F4D-9434-3354390906C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58911314-C104-C84A-B7F5-25DA7D79E696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:N17"/>
+  <dimension ref="B1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -660,8 +660,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.15">
-      <c r="J17" s="2" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B19" s="2" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>